<commit_message>
feat: add code errors, add new tests, new checks in validator
</commit_message>
<xml_diff>
--- a/tests/data/value_in_accumulated_share.xlsx
+++ b/tests/data/value_in_accumulated_share.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WinUser\PycharmProjects\abc_test\pyAnalysis\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5798A5A7-1EB2-4203-9211-7731A8C79CC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D88BBDF-209E-401D-8221-6CE3C9C7C5EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2700" yWindow="1752" windowWidth="17280" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5688" yWindow="2556" windowWidth="17280" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>код идентификатор PLU</t>
   </si>
@@ -70,6 +70,27 @@
   </si>
   <si>
     <t>2.732240</t>
+  </si>
+  <si>
+    <t>81.967213</t>
+  </si>
+  <si>
+    <t>92.896175</t>
+  </si>
+  <si>
+    <t>97.267760</t>
+  </si>
+  <si>
+    <t>Категория</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
@@ -408,15 +429,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="13.109375" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="36.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="36.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -432,8 +457,11 @@
       <c r="E1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -446,8 +474,14 @@
       <c r="D2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -460,8 +494,14 @@
       <c r="D3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -469,13 +509,19 @@
         <v>6</v>
       </c>
       <c r="C4" s="3">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -483,13 +529,19 @@
         <v>7</v>
       </c>
       <c r="C5" s="3">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -502,6 +554,15 @@
       <c r="D6" t="s">
         <v>14</v>
       </c>
+      <c r="E6">
+        <v>150</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C8" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>